<commit_message>
Creazione di nuovi loader. Applicazione del form vertical a tutti i menù di inserimento.
</commit_message>
<xml_diff>
--- a/pages/admin/inserimento/studenti/BaseStudenti.xlsx
+++ b/pages/admin/inserimento/studenti/BaseStudenti.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="132">
   <si>
     <t>CITTA</t>
   </si>
@@ -409,13 +409,19 @@
   </si>
   <si>
     <t>Sleleas@dio.it</t>
+  </si>
+  <si>
+    <t>*                                                                        CAMPO OBBLIGATORIO</t>
+  </si>
+  <si>
+    <t>I CAMPI FACOLTATIVI LASCIATI VUOTI VERRANNO COMPILATI DALLO STUDENTE    O IMPOSATI COME SCONOSCIUTI.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,13 +431,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -462,6 +461,20 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -501,9 +514,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -520,26 +533,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -886,14 +902,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU1165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="8" customWidth="1"/>
     <col min="3" max="3" width="22.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="29.5703125" style="5" customWidth="1"/>
@@ -902,11 +918,11 @@
     <col min="36" max="47" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -915,18 +931,18 @@
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -935,18 +951,25 @@
       <c r="D2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="11" t="s">
         <v>129</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="H2" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -961,13 +984,17 @@
       <c r="F3" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -982,13 +1009,17 @@
       <c r="F4" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+    </row>
+    <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -1003,13 +1034,17 @@
       <c r="F5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+    </row>
+    <row r="6" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1024,13 +1059,17 @@
       <c r="F6" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+    </row>
+    <row r="7" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1043,11 +1082,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+    <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1063,11 +1102,11 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+    <row r="9" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1079,15 +1118,19 @@
       <c r="F9" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="H9" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+    </row>
+    <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1099,15 +1142,17 @@
       <c r="F10" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>102</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1119,15 +1164,17 @@
       <c r="F11" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1139,15 +1186,17 @@
       <c r="F12" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>108</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1159,12 +1208,17 @@
       <c r="F13" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>111</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1177,11 +1231,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>114</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -1197,11 +1251,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>117</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1218,10 +1272,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -1238,10 +1292,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1258,10 +1312,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1275,10 +1329,10 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -1292,10 +1346,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1309,10 +1363,10 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1326,10 +1380,10 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1343,10 +1397,10 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1360,10 +1414,10 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -1377,10 +1431,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="8" t="s">
         <v>95</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1394,10 +1448,10 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>99</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -1414,10 +1468,10 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>103</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -1434,10 +1488,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1454,10 +1508,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>109</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -1474,10 +1528,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="8" t="s">
         <v>112</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1494,10 +1548,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>115</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1511,10 +1565,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="8" t="s">
         <v>118</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1528,10 +1582,10 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>121</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1545,10 +1599,10 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1562,10 +1616,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1579,10 +1633,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1596,10 +1650,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1616,10 +1670,10 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1636,10 +1690,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1656,10 +1710,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1673,10 +1727,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1690,10 +1744,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>96</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1707,10 +1761,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1724,10 +1778,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1741,10 +1795,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="8" t="s">
         <v>107</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1758,10 +1812,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1778,10 +1832,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1798,10 +1852,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>116</v>
       </c>
       <c r="C49" s="1" t="s">
@@ -1815,10 +1869,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="8" t="s">
         <v>119</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1832,10 +1886,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="8" t="s">
         <v>122</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -1849,10 +1903,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1866,10 +1920,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1883,10 +1937,10 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -1900,10 +1954,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C55" s="1" t="s">
@@ -1920,10 +1974,10 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="A56" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1940,10 +1994,10 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="8" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -1960,10 +2014,10 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="8" t="s">
         <v>89</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -1980,10 +2034,10 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -2000,10 +2054,10 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C60" s="1" t="s">
@@ -2020,10 +2074,10 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C61" s="1" t="s">
@@ -2040,10 +2094,10 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="8" t="s">
         <v>66</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -2057,10 +2111,10 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="8" t="s">
         <v>70</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -2074,10 +2128,10 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C64" s="1" t="s">
@@ -2091,10 +2145,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="8" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="1" t="s">
@@ -2108,10 +2162,10 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="8" t="s">
         <v>82</v>
       </c>
       <c r="C66" s="1" t="s">
@@ -2125,10 +2179,10 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="8" t="s">
         <v>86</v>
       </c>
       <c r="C67" s="1" t="s">
@@ -2142,10 +2196,10 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C68" s="1" t="s">
@@ -2159,10 +2213,10 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="8" t="s">
         <v>94</v>
       </c>
       <c r="C69" s="1" t="s">
@@ -2179,10 +2233,10 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="8" t="s">
         <v>98</v>
       </c>
       <c r="C70" s="1" t="s">
@@ -2196,10 +2250,10 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="8" t="s">
         <v>102</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2213,10 +2267,10 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="8" t="s">
         <v>105</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -2230,10 +2284,10 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="8" t="s">
         <v>108</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -2247,10 +2301,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="8" t="s">
         <v>111</v>
       </c>
       <c r="C74" s="1" t="s">
@@ -2264,10 +2318,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="8" t="s">
         <v>114</v>
       </c>
       <c r="C75" s="1" t="s">
@@ -2281,10 +2335,10 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="8" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="1" t="s">
@@ -2298,10 +2352,10 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="8" t="s">
         <v>120</v>
       </c>
       <c r="C77" s="1" t="s">
@@ -2318,10 +2372,10 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="8" t="s">
         <v>123</v>
       </c>
       <c r="C78" s="1" t="s">
@@ -2338,10 +2392,10 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C79" s="1" t="s">
@@ -2358,10 +2412,10 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -2378,10 +2432,10 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C81" s="1" t="s">
@@ -2398,10 +2452,10 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="8" t="s">
         <v>79</v>
       </c>
       <c r="C82" s="1" t="s">
@@ -2418,10 +2472,10 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="8" t="s">
         <v>83</v>
       </c>
       <c r="C83" s="1" t="s">
@@ -2438,10 +2492,10 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C84" s="1" t="s">
@@ -2458,10 +2512,10 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C85" s="1" t="s">
@@ -2478,10 +2532,10 @@
       </c>
     </row>
     <row r="86" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="8" t="s">
         <v>95</v>
       </c>
       <c r="C86" s="1" t="s">
@@ -2498,10 +2552,10 @@
       </c>
     </row>
     <row r="87" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="8" t="s">
         <v>99</v>
       </c>
       <c r="C87" s="1" t="s">
@@ -2518,10 +2572,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="8" t="s">
         <v>103</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -2535,10 +2589,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="8" t="s">
         <v>106</v>
       </c>
       <c r="C89" s="1" t="s">
@@ -2552,10 +2606,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="8" t="s">
         <v>109</v>
       </c>
       <c r="C90" s="1" t="s">
@@ -2569,10 +2623,10 @@
       </c>
     </row>
     <row r="91" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="8" t="s">
         <v>112</v>
       </c>
       <c r="C91" s="1" t="s">
@@ -2586,10 +2640,10 @@
       </c>
     </row>
     <row r="92" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="8" t="s">
         <v>115</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -2603,10 +2657,10 @@
       </c>
     </row>
     <row r="93" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="8" t="s">
         <v>118</v>
       </c>
       <c r="C93" s="1" t="s">
@@ -2617,10 +2671,10 @@
       </c>
     </row>
     <row r="94" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
+      <c r="A94" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="8" t="s">
         <v>121</v>
       </c>
       <c r="C94" s="1" t="s">
@@ -2631,10 +2685,10 @@
       </c>
     </row>
     <row r="95" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="8" t="s">
         <v>124</v>
       </c>
       <c r="C95" s="1" t="s">
@@ -2648,10 +2702,10 @@
       </c>
     </row>
     <row r="96" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
+      <c r="A96" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C96" s="1" t="s">
@@ -2665,10 +2719,10 @@
       </c>
     </row>
     <row r="97" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C97" s="1" t="s">
@@ -2682,10 +2736,10 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C98" s="1" t="s">
@@ -2699,10 +2753,10 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="8" t="s">
         <v>80</v>
       </c>
       <c r="C99" s="1" t="s">
@@ -2716,10 +2770,10 @@
       </c>
     </row>
     <row r="100" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="8" t="s">
         <v>84</v>
       </c>
       <c r="C100" s="1" t="s">
@@ -2733,10 +2787,10 @@
       </c>
     </row>
     <row r="101" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="8" t="s">
         <v>88</v>
       </c>
       <c r="C101" s="1" t="s">
@@ -2753,10 +2807,10 @@
       </c>
     </row>
     <row r="102" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B102" s="8" t="s">
         <v>92</v>
       </c>
       <c r="C102" s="1" t="s">
@@ -2773,10 +2827,10 @@
       </c>
     </row>
     <row r="103" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B103" s="8" t="s">
         <v>96</v>
       </c>
       <c r="C103" s="1" t="s">
@@ -2793,10 +2847,10 @@
       </c>
     </row>
     <row r="104" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
+      <c r="A104" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="8" t="s">
         <v>100</v>
       </c>
       <c r="C104" s="1" t="s">
@@ -2813,10 +2867,10 @@
       </c>
     </row>
     <row r="105" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="11" t="s">
+      <c r="A105" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="8" t="s">
         <v>104</v>
       </c>
       <c r="C105" s="1" t="s">
@@ -2833,10 +2887,10 @@
       </c>
     </row>
     <row r="106" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="11" t="s">
+      <c r="A106" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B106" s="8" t="s">
         <v>107</v>
       </c>
       <c r="C106" s="1" t="s">
@@ -2853,10 +2907,10 @@
       </c>
     </row>
     <row r="107" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
+      <c r="A107" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B107" s="9" t="s">
+      <c r="B107" s="8" t="s">
         <v>110</v>
       </c>
       <c r="C107" s="1" t="s">
@@ -2873,10 +2927,10 @@
       </c>
     </row>
     <row r="108" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
+      <c r="A108" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B108" s="9" t="s">
+      <c r="B108" s="8" t="s">
         <v>113</v>
       </c>
       <c r="C108" s="1" t="s">
@@ -2893,10 +2947,10 @@
       </c>
     </row>
     <row r="109" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="8" t="s">
         <v>116</v>
       </c>
       <c r="C109" s="1" t="s">
@@ -2913,10 +2967,10 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B110" s="8" t="s">
         <v>119</v>
       </c>
       <c r="C110" s="1" t="s">
@@ -2933,10 +2987,10 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
+      <c r="A111" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B111" s="9" t="s">
+      <c r="B111" s="8" t="s">
         <v>122</v>
       </c>
       <c r="C111" s="1" t="s">
@@ -2953,10 +3007,10 @@
       </c>
     </row>
     <row r="112" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="11" t="s">
+      <c r="A112" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B112" s="8" t="s">
         <v>125</v>
       </c>
       <c r="C112" s="1" t="s">
@@ -2973,10 +3027,10 @@
       </c>
     </row>
     <row r="113" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="11" t="s">
+      <c r="A113" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B113" s="9" t="s">
+      <c r="B113" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C113" s="1" t="s">
@@ -2993,10 +3047,10 @@
       </c>
     </row>
     <row r="114" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="11" t="s">
+      <c r="A114" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B114" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C114" s="1" t="s">
@@ -3013,10 +3067,10 @@
       </c>
     </row>
     <row r="115" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="11" t="s">
+      <c r="A115" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B115" s="9" t="s">
+      <c r="B115" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C115" s="1" t="s">
@@ -3033,10 +3087,10 @@
       </c>
     </row>
     <row r="116" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="11" t="s">
+      <c r="A116" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B116" s="8" t="s">
         <v>81</v>
       </c>
       <c r="C116" s="1" t="s">
@@ -3053,10 +3107,10 @@
       </c>
     </row>
     <row r="117" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="11" t="s">
+      <c r="A117" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B117" s="9" t="s">
+      <c r="B117" s="8" t="s">
         <v>85</v>
       </c>
       <c r="C117" s="1" t="s">
@@ -3073,10 +3127,10 @@
       </c>
     </row>
     <row r="118" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="11" t="s">
+      <c r="A118" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="8" t="s">
         <v>89</v>
       </c>
       <c r="C118" s="1" t="s">
@@ -3093,10 +3147,10 @@
       </c>
     </row>
     <row r="119" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="11" t="s">
+      <c r="A119" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B119" s="8" t="s">
         <v>93</v>
       </c>
       <c r="C119" s="1" t="s">
@@ -3113,10 +3167,10 @@
       </c>
     </row>
     <row r="120" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="11" t="s">
+      <c r="A120" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B120" s="9" t="s">
+      <c r="B120" s="8" t="s">
         <v>97</v>
       </c>
       <c r="C120" s="1" t="s">
@@ -3133,10 +3187,10 @@
       </c>
     </row>
     <row r="121" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="11" t="s">
+      <c r="A121" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B121" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C121" s="1" t="s">
@@ -4197,6 +4251,10 @@
     <row r="1164" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1165" ht="30.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H2:L6"/>
+    <mergeCell ref="H9:L13"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>

</xml_diff>